<commit_message>
Fix commas in SYVbT formatting
</commit_message>
<xml_diff>
--- a/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
+++ b/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-eu\InputData\trans\SYVbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\trans\SYVbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D933C4-0A6D-420D-98EC-51C4E8D409F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="9765" tabRatio="923" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="9765" tabRatio="923" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -99,7 +98,7 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -843,23 +842,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="13">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="###0.00_)"/>
-    <numFmt numFmtId="167" formatCode="#,##0_)"/>
-    <numFmt numFmtId="168" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000;\-#,##0.000;&quot;-&quot;"/>
-    <numFmt numFmtId="172" formatCode="#,##0.0;\-#,##0.0;&quot;-&quot;"/>
-    <numFmt numFmtId="173" formatCode="0.000%"/>
-    <numFmt numFmtId="174" formatCode="0.0%;\-0.0%;&quot;-&quot;"/>
-    <numFmt numFmtId="175" formatCode="0.00%;\-0.00%;&quot;-&quot;"/>
-    <numFmt numFmtId="176" formatCode="dd\.mm\.yy"/>
-    <numFmt numFmtId="180" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="###0.00_)"/>
+    <numFmt numFmtId="166" formatCode="#,##0_)"/>
+    <numFmt numFmtId="167" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000;\-#,##0.000;&quot;-&quot;"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0;\-#,##0.0;&quot;-&quot;"/>
+    <numFmt numFmtId="170" formatCode="0.000%"/>
+    <numFmt numFmtId="171" formatCode="0.0%;\-0.0%;&quot;-&quot;"/>
+    <numFmt numFmtId="172" formatCode="0.00%;\-0.00%;&quot;-&quot;"/>
+    <numFmt numFmtId="173" formatCode="dd\.mm\.yy"/>
+    <numFmt numFmtId="174" formatCode="0.0"/>
   </numFmts>
-  <fonts count="57">
+  <fonts count="56">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1176,10 +1175,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial "/>
     </font>
     <font>
       <b/>
@@ -1757,16 +1752,16 @@
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="6">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="6">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="6">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1855,7 +1850,7 @@
     <xf numFmtId="49" fontId="19" fillId="0" borderId="6">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" applyNumberFormat="0">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" applyNumberFormat="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="27" borderId="0">
@@ -1929,28 +1924,28 @@
     <xf numFmtId="0" fontId="41" fillId="30" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="42" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="42" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="31" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="43" fillId="31" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="43" fillId="31" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="29" borderId="21" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="168" fontId="40" fillId="0" borderId="21" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="40" fillId="0" borderId="21" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="29" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="168" fontId="40" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="40" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="40" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="40" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="142" applyFont="1" applyAlignment="1">
@@ -1959,13 +1954,82 @@
     <xf numFmtId="0" fontId="44" fillId="2" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="42" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="42" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="40" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="40" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="40" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="40" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="42" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="43" fillId="31" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="40" fillId="0" borderId="21" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="40" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="40" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="143"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="140" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="141" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="29" borderId="22" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="40" fillId="0" borderId="22" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="29" borderId="23" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="40" fillId="0" borderId="23" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="29" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="29" borderId="7" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="40" fillId="0" borderId="22" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="40" fillId="0" borderId="23" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="46" fillId="2" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="42" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="43" fillId="31" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="40" fillId="0" borderId="22" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="40" fillId="0" borderId="21" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="40" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="40" fillId="0" borderId="23" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="40" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="172" fontId="42" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1974,127 +2038,58 @@
     <xf numFmtId="172" fontId="43" fillId="31" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="172" fontId="40" fillId="0" borderId="22" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="172" fontId="40" fillId="0" borderId="21" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="172" fontId="40" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="40" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="143"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="140" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="141" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="22" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="168" fontId="40" fillId="0" borderId="22" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="23" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="168" fontId="40" fillId="0" borderId="23" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="7" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="172" fontId="40" fillId="0" borderId="22" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="172" fontId="40" fillId="0" borderId="23" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="46" fillId="2" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="42" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="43" fillId="31" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="40" fillId="0" borderId="22" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="40" fillId="0" borderId="21" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="40" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="40" fillId="0" borderId="23" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="40" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="42" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="43" fillId="31" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="40" fillId="0" borderId="22" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="40" fillId="0" borderId="21" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="40" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="40" fillId="0" borderId="23" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="40" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="40" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="31" borderId="20" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="43" fillId="31" borderId="20" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="43" fillId="31" borderId="20" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="31" borderId="21" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="43" fillId="31" borderId="21" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="43" fillId="31" borderId="21" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="43" fillId="31" borderId="20" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="43" fillId="31" borderId="20" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="40" fillId="29" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="40" fillId="29" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="43" fillId="31" borderId="21" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="43" fillId="31" borderId="21" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="42" fillId="30" borderId="19" xfId="141" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="42" fillId="30" borderId="19" xfId="141" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="43" fillId="31" borderId="20" xfId="141" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="43" fillId="31" borderId="20" xfId="141" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="40" fillId="0" borderId="0" xfId="141" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="40" fillId="0" borderId="0" xfId="141" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="43" fillId="31" borderId="21" xfId="141" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="43" fillId="31" borderId="21" xfId="141" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="40" fillId="0" borderId="0" xfId="141" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="40" fillId="0" borderId="0" xfId="141" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="40" fillId="0" borderId="7" xfId="141" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="40" fillId="0" borderId="7" xfId="141" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="29" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2104,7 +2099,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="144" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="24" xfId="144" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="48" fillId="0" borderId="0" xfId="144" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="144" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="7" fillId="0" borderId="0" xfId="144" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="39" fillId="28" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2125,16 +2120,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="52" fillId="28" borderId="25" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="28" borderId="25" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="53" fillId="28" borderId="25" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="52" fillId="28" borderId="25" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="54" fillId="0" borderId="26" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="53" fillId="0" borderId="26" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="29" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="29" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="42" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2143,248 +2138,248 @@
     <xf numFmtId="3" fontId="43" fillId="31" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="29" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="29" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="3" fontId="55" fillId="0" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="54" fillId="0" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="29" borderId="22" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="29" borderId="22" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="3" fontId="55" fillId="0" borderId="22" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="54" fillId="0" borderId="22" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="29" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="29" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="3" fontId="55" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="54" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="29" borderId="7" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="29" borderId="7" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="3" fontId="55" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="54" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="55" fillId="0" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="54" fillId="0" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="55" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="54" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="55" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="54" fillId="0" borderId="7" xfId="142" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="54" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="53" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="54" fillId="33" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="53" fillId="33" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="55" fillId="33" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="54" fillId="33" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="41" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="30" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="30" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="56" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="55" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="30" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="30" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="3" fontId="53" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="52" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="31" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="31" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="3" fontId="55" fillId="31" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="54" fillId="31" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="29" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="29" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="29" borderId="7" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="29" borderId="7" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="33" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="33" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="31" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="31" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="29" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="29" borderId="0" xfId="142" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="29" borderId="7" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="29" borderId="7" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="41" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="41" fillId="30" borderId="19" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="31" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="31" borderId="19" xfId="142" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="40" fillId="29" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="40" fillId="29" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="149">
-    <cellStyle name="20% - Accent1 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Accent1 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Accent2 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Accent3 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Accent4 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Accent5 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Accent6 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Bad 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Calculation 2" xfId="40" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Check Cell 2" xfId="41" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="15"/>
+    <cellStyle name="20% - Accent2 2" xfId="16"/>
+    <cellStyle name="20% - Accent3 2" xfId="17"/>
+    <cellStyle name="20% - Accent4 2" xfId="18"/>
+    <cellStyle name="20% - Accent5 2" xfId="19"/>
+    <cellStyle name="20% - Accent6 2" xfId="20"/>
+    <cellStyle name="40% - Accent1 2" xfId="21"/>
+    <cellStyle name="40% - Accent2 2" xfId="22"/>
+    <cellStyle name="40% - Accent3 2" xfId="23"/>
+    <cellStyle name="40% - Accent4 2" xfId="24"/>
+    <cellStyle name="40% - Accent5 2" xfId="25"/>
+    <cellStyle name="40% - Accent6 2" xfId="26"/>
+    <cellStyle name="60% - Accent1 2" xfId="27"/>
+    <cellStyle name="60% - Accent2 2" xfId="28"/>
+    <cellStyle name="60% - Accent3 2" xfId="29"/>
+    <cellStyle name="60% - Accent4 2" xfId="30"/>
+    <cellStyle name="60% - Accent5 2" xfId="31"/>
+    <cellStyle name="60% - Accent6 2" xfId="32"/>
+    <cellStyle name="Accent1 2" xfId="33"/>
+    <cellStyle name="Accent2 2" xfId="34"/>
+    <cellStyle name="Accent3 2" xfId="35"/>
+    <cellStyle name="Accent4 2" xfId="36"/>
+    <cellStyle name="Accent5 2" xfId="37"/>
+    <cellStyle name="Accent6 2" xfId="38"/>
+    <cellStyle name="Bad 2" xfId="39"/>
+    <cellStyle name="Body: normal cell" xfId="4"/>
+    <cellStyle name="Calculation 2" xfId="40"/>
+    <cellStyle name="Check Cell 2" xfId="41"/>
     <cellStyle name="Comma" xfId="140" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Comma 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Comma 2 2 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Comma 2 2 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Comma 2 3" xfId="45" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Comma 3" xfId="46" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Comma 4" xfId="47" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Comma 5" xfId="48" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Comma 6" xfId="49" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Comma 7" xfId="50" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Currency 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Currency 3" xfId="52" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Currency 3 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Data" xfId="54" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Data no deci" xfId="55" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Data Superscript" xfId="56" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="57" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="2" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Good 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Heading 1 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Heading 2 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Heading 3 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Heading 4 2" xfId="63" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Hed Side" xfId="13" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Hed Side bold" xfId="64" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Hed Side Indent" xfId="65" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Hed Side Regular" xfId="66" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="67" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Hed Top" xfId="68" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Comma 2" xfId="42"/>
+    <cellStyle name="Comma 2 2" xfId="11"/>
+    <cellStyle name="Comma 2 2 2" xfId="43"/>
+    <cellStyle name="Comma 2 2 3" xfId="44"/>
+    <cellStyle name="Comma 2 3" xfId="45"/>
+    <cellStyle name="Comma 3" xfId="46"/>
+    <cellStyle name="Comma 4" xfId="47"/>
+    <cellStyle name="Comma 5" xfId="48"/>
+    <cellStyle name="Comma 6" xfId="49"/>
+    <cellStyle name="Comma 7" xfId="50"/>
+    <cellStyle name="Currency 2" xfId="51"/>
+    <cellStyle name="Currency 3" xfId="52"/>
+    <cellStyle name="Currency 3 2" xfId="53"/>
+    <cellStyle name="Data" xfId="54"/>
+    <cellStyle name="Data no deci" xfId="55"/>
+    <cellStyle name="Data Superscript" xfId="56"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="57"/>
+    <cellStyle name="Explanatory Text 2" xfId="58"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="6"/>
+    <cellStyle name="Footnotes: top row" xfId="2"/>
+    <cellStyle name="Good 2" xfId="59"/>
+    <cellStyle name="Header: bottom row" xfId="5"/>
+    <cellStyle name="Heading 1 2" xfId="60"/>
+    <cellStyle name="Heading 2 2" xfId="61"/>
+    <cellStyle name="Heading 3 2" xfId="62"/>
+    <cellStyle name="Heading 4 2" xfId="63"/>
+    <cellStyle name="Hed Side" xfId="13"/>
+    <cellStyle name="Hed Side bold" xfId="64"/>
+    <cellStyle name="Hed Side Indent" xfId="65"/>
+    <cellStyle name="Hed Side Regular" xfId="66"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="67"/>
+    <cellStyle name="Hed Top" xfId="68"/>
     <cellStyle name="Hyperlink" xfId="143" builtinId="8"/>
-    <cellStyle name="Input 2" xfId="69" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Neutral 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Input 2" xfId="69"/>
+    <cellStyle name="Linked Cell 2" xfId="70"/>
+    <cellStyle name="Neutral 2" xfId="71"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="72" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Normal 11" xfId="10" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Normal 2 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Normal 2 2 2" xfId="74" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Normal 2 2 3" xfId="75" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Normal 2 3" xfId="76" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Normal 2 4" xfId="77" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 2 5" xfId="142" xr:uid="{1BD59478-1179-44CD-AB5B-99ECC9626B09}"/>
-    <cellStyle name="Normal 3" xfId="8" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 3 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="79" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="80" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="81" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Normal 3 3" xfId="82" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Normal 3 3 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Normal 3 4" xfId="86" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Normal 3 4 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Normal 3 5" xfId="88" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Normal 3 6" xfId="89" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Normal 3 7" xfId="90" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 3 8" xfId="91" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 3 9" xfId="12" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 4" xfId="92" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 4 2" xfId="93" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Normal 4 2 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Normal 4 2 3" xfId="96" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Normal 4 3" xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Normal 4 3 2" xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="99" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Normal 4 3 3" xfId="100" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Normal 4 4" xfId="101" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 4 4 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 4 5" xfId="103" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 4 6" xfId="104" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 4 7" xfId="105" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 4 8" xfId="106" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 5" xfId="107" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 5 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 5 3" xfId="109" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 6" xfId="110" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 6 2" xfId="111" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 7" xfId="112" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 8" xfId="113" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 9" xfId="114" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Note 2" xfId="115" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Note 2 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Output 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Normal 10" xfId="72"/>
+    <cellStyle name="Normal 11" xfId="10"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="73"/>
+    <cellStyle name="Normal 2 2 2" xfId="74"/>
+    <cellStyle name="Normal 2 2 3" xfId="75"/>
+    <cellStyle name="Normal 2 3" xfId="76"/>
+    <cellStyle name="Normal 2 4" xfId="77"/>
+    <cellStyle name="Normal 2 5" xfId="142"/>
+    <cellStyle name="Normal 3" xfId="8"/>
+    <cellStyle name="Normal 3 2" xfId="78"/>
+    <cellStyle name="Normal 3 2 2" xfId="79"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="80"/>
+    <cellStyle name="Normal 3 2 3" xfId="81"/>
+    <cellStyle name="Normal 3 3" xfId="82"/>
+    <cellStyle name="Normal 3 3 2" xfId="83"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="84"/>
+    <cellStyle name="Normal 3 3 3" xfId="85"/>
+    <cellStyle name="Normal 3 4" xfId="86"/>
+    <cellStyle name="Normal 3 4 2" xfId="87"/>
+    <cellStyle name="Normal 3 5" xfId="88"/>
+    <cellStyle name="Normal 3 6" xfId="89"/>
+    <cellStyle name="Normal 3 7" xfId="90"/>
+    <cellStyle name="Normal 3 8" xfId="91"/>
+    <cellStyle name="Normal 3 9" xfId="12"/>
+    <cellStyle name="Normal 4" xfId="92"/>
+    <cellStyle name="Normal 4 2" xfId="93"/>
+    <cellStyle name="Normal 4 2 2" xfId="94"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="95"/>
+    <cellStyle name="Normal 4 2 3" xfId="96"/>
+    <cellStyle name="Normal 4 3" xfId="97"/>
+    <cellStyle name="Normal 4 3 2" xfId="98"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="99"/>
+    <cellStyle name="Normal 4 3 3" xfId="100"/>
+    <cellStyle name="Normal 4 4" xfId="101"/>
+    <cellStyle name="Normal 4 4 2" xfId="102"/>
+    <cellStyle name="Normal 4 5" xfId="103"/>
+    <cellStyle name="Normal 4 6" xfId="104"/>
+    <cellStyle name="Normal 4 7" xfId="105"/>
+    <cellStyle name="Normal 4 8" xfId="106"/>
+    <cellStyle name="Normal 5" xfId="107"/>
+    <cellStyle name="Normal 5 2" xfId="108"/>
+    <cellStyle name="Normal 5 3" xfId="109"/>
+    <cellStyle name="Normal 6" xfId="110"/>
+    <cellStyle name="Normal 6 2" xfId="111"/>
+    <cellStyle name="Normal 7" xfId="112"/>
+    <cellStyle name="Normal 8" xfId="113"/>
+    <cellStyle name="Normal 9" xfId="114"/>
+    <cellStyle name="Note 2" xfId="115"/>
+    <cellStyle name="Note 2 2" xfId="116"/>
+    <cellStyle name="Output 2" xfId="117"/>
+    <cellStyle name="Parent row" xfId="3"/>
     <cellStyle name="Percent" xfId="141" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Percent 2 2" xfId="119" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Percent 3" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Percent 3 2" xfId="121" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Prozent 2" xfId="148" xr:uid="{34DDAA79-0950-4E12-A733-1B81120079C7}"/>
-    <cellStyle name="Source Hed" xfId="122" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Source Superscript" xfId="123" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Source Text" xfId="9" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Standard 2" xfId="144" xr:uid="{DAF255F9-941A-43FE-ABD4-6FCDF68F3B0A}"/>
-    <cellStyle name="Standard 3" xfId="145" xr:uid="{FD2AB7E4-9B4A-437F-B310-4BE6FCCF71A5}"/>
-    <cellStyle name="Standard 4" xfId="146" xr:uid="{00DB1AA1-CAF2-49EC-86B5-EC72264E2FD6}"/>
-    <cellStyle name="Standard 5" xfId="147" xr:uid="{26A0622A-7B3B-4B48-99C0-D38073ECB0F5}"/>
-    <cellStyle name="State" xfId="124" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Superscript" xfId="125" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Table Data" xfId="126" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Table Head Top" xfId="127" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Table Hed Side" xfId="128" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Table title" xfId="7" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Title 2" xfId="129" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Title Text" xfId="130" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Title Text 1" xfId="131" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Title Text 2" xfId="132" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Title-1" xfId="14" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Title-2" xfId="133" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Title-3" xfId="134" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Total 2" xfId="135" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Warning Text 2" xfId="136" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Wrap" xfId="137" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Wrap Bold" xfId="138" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Wrap Title" xfId="139" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Percent 2" xfId="118"/>
+    <cellStyle name="Percent 2 2" xfId="119"/>
+    <cellStyle name="Percent 3" xfId="120"/>
+    <cellStyle name="Percent 3 2" xfId="121"/>
+    <cellStyle name="Prozent 2" xfId="148"/>
+    <cellStyle name="Source Hed" xfId="122"/>
+    <cellStyle name="Source Superscript" xfId="123"/>
+    <cellStyle name="Source Text" xfId="9"/>
+    <cellStyle name="Standard 2" xfId="144"/>
+    <cellStyle name="Standard 3" xfId="145"/>
+    <cellStyle name="Standard 4" xfId="146"/>
+    <cellStyle name="Standard 5" xfId="147"/>
+    <cellStyle name="State" xfId="124"/>
+    <cellStyle name="Superscript" xfId="125"/>
+    <cellStyle name="Table Data" xfId="126"/>
+    <cellStyle name="Table Head Top" xfId="127"/>
+    <cellStyle name="Table Hed Side" xfId="128"/>
+    <cellStyle name="Table title" xfId="7"/>
+    <cellStyle name="Title 2" xfId="129"/>
+    <cellStyle name="Title Text" xfId="130"/>
+    <cellStyle name="Title Text 1" xfId="131"/>
+    <cellStyle name="Title Text 2" xfId="132"/>
+    <cellStyle name="Title-1" xfId="14"/>
+    <cellStyle name="Title-2" xfId="133"/>
+    <cellStyle name="Title-3" xfId="134"/>
+    <cellStyle name="Total 2" xfId="135"/>
+    <cellStyle name="Warning Text 2" xfId="136"/>
+    <cellStyle name="Wrap" xfId="137"/>
+    <cellStyle name="Wrap Bold" xfId="138"/>
+    <cellStyle name="Wrap Title" xfId="139"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2920,23 +2915,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2972,23 +2950,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3164,16 +3125,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="77.58984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3579,17 +3540,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B69" r:id="rId1" xr:uid="{57410C99-DBA1-45A0-A3FF-452AE1731FF0}"/>
-    <hyperlink ref="B62" r:id="rId2" xr:uid="{BCA42AD9-5992-44CD-9664-27674A1AC99D}"/>
-    <hyperlink ref="B49" r:id="rId3" xr:uid="{5B92F5FD-E8D4-41BC-BD9B-2FD1E8358EF7}"/>
-    <hyperlink ref="B7" r:id="rId4" xr:uid="{1B6A0A43-A054-4211-A622-24F7DD6581CE}"/>
-    <hyperlink ref="B21" r:id="rId5" xr:uid="{C8557EB3-9D98-4884-837E-D60B84311F35}"/>
-    <hyperlink ref="B28" r:id="rId6" xr:uid="{8D1C20C8-4702-4552-A612-A1A08D2C9721}"/>
-    <hyperlink ref="B14" r:id="rId7" xr:uid="{50E5846A-4DDA-49A2-BA1F-2980BE32DE5F}"/>
-    <hyperlink ref="B42" r:id="rId8" xr:uid="{77598C45-A77B-42EB-8F4F-391EAA572C06}"/>
-    <hyperlink ref="B35" r:id="rId9" xr:uid="{EE9A67DE-C38F-4801-9B1B-3EBE5E16A800}"/>
-    <hyperlink ref="A84" r:id="rId10" xr:uid="{5446C9BD-43B8-4A5B-A99B-229723C1715D}"/>
-    <hyperlink ref="B56" r:id="rId11" xr:uid="{AFA4FBF4-505E-444E-A397-3D050C25871C}"/>
+    <hyperlink ref="B69" r:id="rId1"/>
+    <hyperlink ref="B62" r:id="rId2"/>
+    <hyperlink ref="B49" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B21" r:id="rId5"/>
+    <hyperlink ref="B28" r:id="rId6"/>
+    <hyperlink ref="B14" r:id="rId7"/>
+    <hyperlink ref="B42" r:id="rId8"/>
+    <hyperlink ref="B35" r:id="rId9"/>
+    <hyperlink ref="A84" r:id="rId10"/>
+    <hyperlink ref="B56" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>
@@ -3597,13 +3558,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB616C29-F7FC-4EFF-9E75-476B4EFF7F2C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:S135"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
@@ -3613,8 +3574,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="50.7265625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.7265625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="50.73046875" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.73046875" style="21" customWidth="1"/>
     <col min="18" max="16384" width="9.1328125" style="11"/>
   </cols>
   <sheetData>
@@ -11052,7 +11013,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10BA1A4-7D9B-4BED-AE12-6AA113D6E293}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -11068,10 +11029,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="50.7265625" style="11" customWidth="1"/>
-    <col min="2" max="10" width="10.7265625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="50.73046875" style="11" customWidth="1"/>
+    <col min="2" max="10" width="10.73046875" style="21" customWidth="1"/>
     <col min="11" max="11" width="14.1328125" style="21" customWidth="1"/>
-    <col min="12" max="17" width="10.7265625" style="21" customWidth="1"/>
+    <col min="12" max="17" width="10.73046875" style="21" customWidth="1"/>
     <col min="18" max="16384" width="9.1328125" style="11"/>
   </cols>
   <sheetData>
@@ -12180,7 +12141,7 @@
       </c>
       <c r="M26" s="83"/>
     </row>
-    <row r="27" spans="1:18" ht="14.75">
+    <row r="27" spans="1:18" ht="14.25">
       <c r="A27" s="75" t="s">
         <v>157</v>
       </c>
@@ -13031,7 +12992,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19959718-0CD7-445B-9681-74AA6132390D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -13044,8 +13005,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="50.7265625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.7265625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="50.73046875" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.73046875" style="21" customWidth="1"/>
     <col min="18" max="16384" width="9.1328125" style="11"/>
   </cols>
   <sheetData>
@@ -15230,7 +15191,7 @@
         <f t="shared" si="18"/>
         <v>8346.0790641255444</v>
       </c>
-      <c r="S40" s="123">
+      <c r="S40" s="122">
         <f>AVERAGE(L40:Q40)</f>
         <v>8271.5546728681056</v>
       </c>
@@ -15462,7 +15423,7 @@
         <f t="shared" si="19"/>
         <v>507.99873350961605</v>
       </c>
-      <c r="S44" s="123">
+      <c r="S44" s="122">
         <f>AVERAGE(L44:Q44)</f>
         <v>499.94334089238419</v>
       </c>
@@ -19444,14 +19405,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EFC385B-2769-4081-AB3F-062F9A7FB117}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -19838,7 +19799,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{B6FFE004-BD37-406B-B680-558CB33EE819}"/>
+    <hyperlink ref="A4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
@@ -19846,20 +19807,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F8A45B-496F-4B4D-8B9D-B6C9BE580EE8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="46.7265625" customWidth="1"/>
+    <col min="1" max="1" width="46.73046875" customWidth="1"/>
     <col min="3" max="4" width="15.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.40625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20607,8 +20568,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{D5350A30-2F48-4685-B726-B62FF0E20379}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{D625FC42-3AFF-46BA-9C32-A86DA6474159}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -20616,7 +20577,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F0CD08-F62A-46CA-AF75-3076583F1BDC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ251"/>
   <sheetViews>
     <sheetView topLeftCell="A196" workbookViewId="0">
@@ -20624,14 +20585,14 @@
       <selection pane="topRight" activeCell="Q111" sqref="Q111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="46.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.04296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="52" width="9.04296875" customWidth="1"/>
+    <col min="1" max="1" width="46.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="52" width="9.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="15.5" thickBot="1">
+    <row r="1" spans="1:52" ht="14.65" thickBot="1">
       <c r="A1" s="87" t="s">
         <v>192</v>
       </c>
@@ -55625,7 +55586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -55635,18 +55596,18 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="16.86328125" customWidth="1"/>
-    <col min="2" max="2" width="24.58984375" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" customWidth="1"/>
     <col min="3" max="3" width="20.86328125" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" customWidth="1"/>
+    <col min="4" max="4" width="18.265625" customWidth="1"/>
     <col min="5" max="5" width="17.1328125" customWidth="1"/>
-    <col min="6" max="8" width="23.26953125" customWidth="1"/>
-    <col min="10" max="10" width="14.40625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="23.265625" customWidth="1"/>
+    <col min="10" max="10" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29.5">
+    <row r="1" spans="1:8">
       <c r="A1" s="84" t="s">
         <v>18</v>
       </c>
@@ -55852,29 +55813,29 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="16.86328125" customWidth="1"/>
-    <col min="2" max="2" width="24.58984375" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" customWidth="1"/>
     <col min="3" max="3" width="20.86328125" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" customWidth="1"/>
+    <col min="4" max="4" width="18.265625" customWidth="1"/>
     <col min="5" max="5" width="17.1328125" customWidth="1"/>
-    <col min="6" max="8" width="23.26953125" customWidth="1"/>
-    <col min="9" max="9" width="13.40625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.58984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="23.265625" customWidth="1"/>
+    <col min="9" max="9" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29.5">
+    <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -55904,31 +55865,31 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="122">
+      <c r="B2" s="123">
         <f>TRA_StockTot!U134</f>
         <v>94943</v>
       </c>
-      <c r="C2" s="122">
+      <c r="C2" s="123">
         <f>TRA_StockTot!U113</f>
         <v>159546</v>
       </c>
-      <c r="D2" s="122">
+      <c r="D2" s="123">
         <f>TRA_StockTot!U112</f>
         <v>2339955</v>
       </c>
-      <c r="E2" s="122">
+      <c r="E2" s="123">
         <f>TRA_StockTot!U115</f>
         <v>28855073</v>
       </c>
-      <c r="F2" s="122">
+      <c r="F2" s="123">
         <f>TRA_StockTot!U126</f>
         <v>65102</v>
       </c>
-      <c r="G2" s="122">
+      <c r="G2" s="123">
         <f>TRA_StockTot!U111</f>
         <v>292214</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="123">
         <f>'Alternative Fuel Vehicles'!B28</f>
         <v>296</v>
       </c>
@@ -55937,30 +55898,30 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="123">
         <f>'Alternative Fuel Vehicles'!C12</f>
         <v>284</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="123">
         <f>SUM('Alternative Fuel Vehicles'!E12:F12)</f>
         <v>21446</v>
       </c>
-      <c r="D3" s="122">
+      <c r="D3" s="123">
         <f>TRA_StockTot!U145+TRA_StockTot!U164</f>
         <v>33</v>
       </c>
-      <c r="E3" s="122">
+      <c r="E3" s="123">
         <f>TRA_StockTot!U144+TRA_StockTot!U163</f>
         <v>6794192</v>
       </c>
-      <c r="F3" s="8">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8">
+      <c r="F3" s="123">
+        <v>0</v>
+      </c>
+      <c r="G3" s="123">
         <f>'Alternative Fuel Vehicles'!G12</f>
         <v>0</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="123">
         <f>'Alternative Fuel Vehicles'!B12</f>
         <v>6</v>
       </c>
@@ -55969,26 +55930,26 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="B4" s="123">
+        <v>0</v>
+      </c>
+      <c r="C4" s="123">
+        <v>0</v>
+      </c>
+      <c r="D4" s="123">
+        <v>0</v>
+      </c>
+      <c r="E4" s="123">
         <f>TrAvia_act!S44</f>
         <v>499.94334089238419</v>
       </c>
-      <c r="F4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4" s="8">
-        <v>0</v>
-      </c>
-      <c r="H4" s="8">
+      <c r="F4" s="123">
+        <v>0</v>
+      </c>
+      <c r="G4" s="123">
+        <v>0</v>
+      </c>
+      <c r="H4" s="123">
         <v>0</v>
       </c>
     </row>
@@ -55996,27 +55957,27 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="122">
+      <c r="B5" s="123">
         <f>TRA_StockTot!U190</f>
         <v>4566.3906058589173</v>
       </c>
-      <c r="C5" s="8">
-        <v>0</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="122">
+      <c r="C5" s="123">
+        <v>0</v>
+      </c>
+      <c r="D5" s="123">
+        <v>0</v>
+      </c>
+      <c r="E5" s="123">
         <f>TRA_StockTot!U189</f>
         <v>1661.0121017769959</v>
       </c>
-      <c r="F5" s="8">
-        <v>0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8">
+      <c r="F5" s="123">
+        <v>0</v>
+      </c>
+      <c r="G5" s="123">
+        <v>0</v>
+      </c>
+      <c r="H5" s="123">
         <v>0</v>
       </c>
     </row>
@@ -56024,26 +55985,26 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8">
-        <v>0</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0</v>
-      </c>
-      <c r="D6" s="8">
-        <v>0</v>
-      </c>
-      <c r="E6" s="122">
+      <c r="B6" s="123">
+        <v>0</v>
+      </c>
+      <c r="C6" s="123">
+        <v>0</v>
+      </c>
+      <c r="D6" s="123">
+        <v>0</v>
+      </c>
+      <c r="E6" s="123">
         <f>TRA_StockTot!U223+TRA_StockTot!U230+TRA_StockTot!U239+TRA_StockTot!U246</f>
         <v>4077.5125867167935</v>
       </c>
-      <c r="F6" s="8">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="F6" s="123">
+        <v>0</v>
+      </c>
+      <c r="G6" s="123">
+        <v>0</v>
+      </c>
+      <c r="H6" s="123">
         <v>0</v>
       </c>
     </row>
@@ -56051,25 +56012,25 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8">
+      <c r="B7" s="123">
+        <v>0</v>
+      </c>
+      <c r="C7" s="123">
+        <v>0</v>
+      </c>
+      <c r="D7" s="123">
+        <v>0</v>
+      </c>
+      <c r="E7" s="123">
+        <v>0</v>
+      </c>
+      <c r="F7" s="123">
+        <v>0</v>
+      </c>
+      <c r="G7" s="123">
+        <v>0</v>
+      </c>
+      <c r="H7" s="123">
         <v>0</v>
       </c>
     </row>
@@ -56084,6 +56045,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="C3" formulaRange="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Adds intra-EU, international airplane stock
</commit_message>
<xml_diff>
--- a/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
+++ b/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\trans\SYVbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\SYVbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1781FD-DCA6-4309-B143-18F2EC742918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5CC78E-CB2D-4DB1-9FFD-CA20CAC1B1AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5880" windowWidth="38640" windowHeight="21120" tabRatio="744" firstSheet="1" activeTab="6" xr2:uid="{05A92713-FF8C-4705-B0D9-268054C6A6B1}"/>
+    <workbookView xWindow="32250" yWindow="1470" windowWidth="25020" windowHeight="12165" tabRatio="744" firstSheet="1" activeTab="6" xr2:uid="{05A92713-FF8C-4705-B0D9-268054C6A6B1}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1939,8 +1939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357CB24D-1D6B-4122-9DA1-45BAC6D526D4}">
   <dimension ref="A1:E120"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53116,8 +53116,8 @@
   </sheetPr>
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53419,8 +53419,8 @@
         <v>0</v>
       </c>
       <c r="E8" s="73">
-        <f>'Raw data JRC Aircraft'!E41</f>
-        <v>136.969297198725</v>
+        <f>'Raw data JRC Aircraft'!E41+'Raw data JRC Aircraft'!E42</f>
+        <v>770.012089991518</v>
       </c>
       <c r="F8" s="73">
         <v>0</v>
@@ -53430,7 +53430,7 @@
       </c>
       <c r="H8" s="73">
         <f>('Raw data JRC Aircraft'!E41+'Raw data JRC Aircraft'!E42)-SUM(B8:G8)</f>
-        <v>633.04279279279297</v>
+        <v>0</v>
       </c>
       <c r="I8" s="136">
         <f t="shared" si="0"/>
@@ -53885,8 +53885,8 @@
         <v>0</v>
       </c>
       <c r="E17" s="73">
-        <f>'Raw data JRC Aircraft'!B31</f>
-        <v>1103.3234132134789</v>
+        <f>'Raw data JRC Aircraft'!B31+'Raw data JRC Aircraft'!B32</f>
+        <v>4828.8394913743059</v>
       </c>
       <c r="F17" s="73">
         <v>0</v>
@@ -53899,7 +53899,7 @@
       </c>
       <c r="I17" s="136">
         <f t="shared" si="2"/>
-        <v>1103.3234132134789</v>
+        <v>4828.8394913743059</v>
       </c>
       <c r="L17" s="126" t="s">
         <v>147</v>
@@ -54352,7 +54352,7 @@
       </c>
       <c r="E26" s="115">
         <f>IFERROR(E8/E17,0)</f>
-        <v>0.12414247314828186</v>
+        <v>0.15946110682845863</v>
       </c>
       <c r="F26" s="115">
         <f t="shared" si="9"/>
@@ -54368,7 +54368,7 @@
       </c>
       <c r="I26" s="115">
         <f t="shared" si="7"/>
-        <v>0.6979024289431357</v>
+        <v>0.15946110682845863</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>147</v>
@@ -54853,7 +54853,7 @@
       </c>
       <c r="E37" s="73">
         <f t="shared" si="19"/>
-        <v>1103.3234132134789</v>
+        <v>4828.8394913743059</v>
       </c>
       <c r="F37" s="73">
         <f t="shared" si="19"/>
@@ -54869,7 +54869,7 @@
       </c>
       <c r="I37" s="136">
         <f t="shared" si="17"/>
-        <v>1103.3234132134789</v>
+        <v>4828.8394913743059</v>
       </c>
       <c r="J37" s="129" t="s">
         <v>156</v>
@@ -55334,7 +55334,7 @@
       </c>
       <c r="E47" s="73">
         <f t="shared" si="27"/>
-        <v>966.35411601475391</v>
+        <v>4058.8274013827881</v>
       </c>
       <c r="F47" s="73">
         <f t="shared" si="27"/>
@@ -55350,7 +55350,7 @@
       </c>
       <c r="I47" s="136">
         <f t="shared" si="25"/>
-        <v>966.35411601475391</v>
+        <v>4058.8274013827881</v>
       </c>
       <c r="L47" s="131" t="s">
         <v>147</v>
@@ -55880,7 +55880,7 @@
       </c>
       <c r="E4" s="144">
         <f>Calculations!E47</f>
-        <v>966.35411601475391</v>
+        <v>4058.8274013827881</v>
       </c>
       <c r="F4" s="144">
         <f>Calculations!F47</f>
@@ -56251,6 +56251,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
@@ -56259,15 +56268,6 @@
     <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -56494,20 +56494,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B958747-05AB-4C5B-933F-03EB048ECECF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D86501B8-0259-48A1-9C13-881AE5763A57}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
     <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B958747-05AB-4C5B-933F-03EB048ECECF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>